<commit_message>
added the 4 previously missing DAT1 3'UTR genotypes
</commit_message>
<xml_diff>
--- a/Analyses Scripts_R/DAT1genotypes_forR.xlsx
+++ b/Analyses Scripts_R/DAT1genotypes_forR.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="117">
   <si>
     <t>ID</t>
   </si>
@@ -1178,8 +1178,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D102"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="A81" sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1822,6 +1822,9 @@
       <c r="A47" t="s">
         <v>58</v>
       </c>
+      <c r="B47" t="s">
+        <v>13</v>
+      </c>
       <c r="D47" t="s">
         <v>7</v>
       </c>
@@ -2040,6 +2043,9 @@
       <c r="A63" t="s">
         <v>75</v>
       </c>
+      <c r="B63" t="s">
+        <v>5</v>
+      </c>
       <c r="C63" t="s">
         <v>6</v>
       </c>
@@ -2275,6 +2281,9 @@
       <c r="A80" t="s">
         <v>93</v>
       </c>
+      <c r="B80" t="s">
+        <v>13</v>
+      </c>
       <c r="D80" t="s">
         <v>7</v>
       </c>
@@ -2282,6 +2291,9 @@
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>94</v>
+      </c>
+      <c r="B81" t="s">
+        <v>13</v>
       </c>
       <c r="D81" t="s">
         <v>7</v>

</xml_diff>